<commit_message>
B-Em breakpoint and debug output added
</commit_message>
<xml_diff>
--- a/Memory differences Level 20 vs assembly.xlsx
+++ b/Memory differences Level 20 vs assembly.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\BirdStrike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B1D9FACD-EE42-40B5-AE2A-C5043BD74D3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A57C30-6902-4B82-B7DC-A2F664F1D5B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="18000" windowHeight="9397" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="l20vsOrig" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
   <si>
     <t>A9</t>
   </si>
@@ -338,12 +338,18 @@
   </si>
   <si>
     <t>Prevents player movement</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>(level 23)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1183,11 +1189,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D49" sqref="D48:D49"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2451,6 +2457,20 @@
         <v>c 2D7F 0</v>
       </c>
     </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B57" s="1">
+        <v>2852</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>